<commit_message>
add human readable title to xlsx init
</commit_message>
<xml_diff>
--- a/bin/init/table.xlsx
+++ b/bin/init/table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Const" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="33">
   <si>
     <t>on</t>
   </si>
@@ -66,6 +66,57 @@
   </si>
   <si>
     <t>modifiers</t>
+  </si>
+  <si>
+    <t>Rate Law</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Rule</t>
+  </si>
+  <si>
+    <t>Initial Value</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Space</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Boundary</t>
+  </si>
+  <si>
+    <t>Spae</t>
+  </si>
+  <si>
+    <t>Compartment</t>
+  </si>
+  <si>
+    <t>Is Amount</t>
+  </si>
+  <si>
+    <t>Modifiers</t>
+  </si>
+  <si>
+    <t>Reaction Expression</t>
   </si>
 </sst>
 </file>
@@ -99,7 +150,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,6 +160,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -134,11 +191,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -442,13 +500,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.7265625" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -480,9 +538,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -491,7 +576,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -540,7 +625,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -551,7 +667,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -593,7 +709,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -604,7 +751,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -654,7 +801,44 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -664,14 +848,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="5" max="5" width="18.54296875" customWidth="1"/>
     <col min="6" max="6" width="9.54296875" customWidth="1"/>
+    <col min="7" max="7" width="19.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
@@ -706,7 +891,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>